<commit_message>
Update input setup for storage China
</commit_message>
<xml_diff>
--- a/scenario work/China/data/setup_storage_CHN.xlsx
+++ b/scenario work/China/data/setup_storage_CHN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakeri\Documents\Github\time_clustering\scenario work\China\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE13B96-0DD9-4ED4-A55A-BBD3ABE029CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6969DCD-98DD-41F0-BFA1-7A7F0F561218}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="71">
   <si>
     <t>technology</t>
   </si>
@@ -536,22 +536,13 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -572,13 +563,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -887,14 +887,14 @@
   <dimension ref="A1:W28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.85546875" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
@@ -995,7 +995,9 @@
       <c r="C2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="E2" s="5" t="s">
         <v>27</v>
       </c>
@@ -1042,7 +1044,7 @@
       </c>
       <c r="U2" s="5"/>
       <c r="V2" s="5"/>
-      <c r="W2" s="84" t="s">
+      <c r="W2" s="81" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1109,7 +1111,7 @@
       <c r="V3" s="12">
         <v>0.01</v>
       </c>
-      <c r="W3" s="85"/>
+      <c r="W3" s="82"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1121,7 +1123,9 @@
       <c r="C4" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>53</v>
+      </c>
       <c r="E4" s="9" t="s">
         <v>27</v>
       </c>
@@ -1170,7 +1174,7 @@
       </c>
       <c r="U4" s="9"/>
       <c r="V4" s="12"/>
-      <c r="W4" s="86"/>
+      <c r="W4" s="83"/>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
@@ -1182,7 +1186,9 @@
       <c r="C5" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="31"/>
+      <c r="D5" s="31" t="s">
+        <v>53</v>
+      </c>
       <c r="E5" s="31" t="s">
         <v>27</v>
       </c>
@@ -1229,7 +1235,7 @@
       </c>
       <c r="U5" s="31"/>
       <c r="V5" s="31"/>
-      <c r="W5" s="90" t="s">
+      <c r="W5" s="78" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1296,7 +1302,7 @@
       <c r="V6" s="40">
         <v>0.01</v>
       </c>
-      <c r="W6" s="91"/>
+      <c r="W6" s="79"/>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="s">
@@ -1308,7 +1314,9 @@
       <c r="C7" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D7" s="42"/>
+      <c r="D7" s="42" t="s">
+        <v>53</v>
+      </c>
       <c r="E7" s="42" t="s">
         <v>27</v>
       </c>
@@ -1357,7 +1365,7 @@
       </c>
       <c r="U7" s="42"/>
       <c r="V7" s="42"/>
-      <c r="W7" s="92"/>
+      <c r="W7" s="80"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
@@ -1369,7 +1377,9 @@
       <c r="C8" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="31"/>
+      <c r="D8" s="31" t="s">
+        <v>53</v>
+      </c>
       <c r="E8" s="31" t="s">
         <v>27</v>
       </c>
@@ -1416,7 +1426,7 @@
       </c>
       <c r="U8" s="31"/>
       <c r="V8" s="31"/>
-      <c r="W8" s="90" t="s">
+      <c r="W8" s="78" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1483,7 +1493,7 @@
       <c r="V9" s="40">
         <v>0.01</v>
       </c>
-      <c r="W9" s="91"/>
+      <c r="W9" s="79"/>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="42" t="s">
@@ -1495,7 +1505,9 @@
       <c r="C10" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="42"/>
+      <c r="D10" s="42" t="s">
+        <v>53</v>
+      </c>
       <c r="E10" s="42" t="s">
         <v>27</v>
       </c>
@@ -1544,7 +1556,7 @@
       </c>
       <c r="U10" s="42"/>
       <c r="V10" s="42"/>
-      <c r="W10" s="92"/>
+      <c r="W10" s="80"/>
     </row>
     <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
@@ -1556,7 +1568,9 @@
       <c r="C11" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="31"/>
+      <c r="D11" s="31" t="s">
+        <v>53</v>
+      </c>
       <c r="E11" s="31" t="s">
         <v>27</v>
       </c>
@@ -1603,7 +1617,7 @@
       </c>
       <c r="U11" s="31"/>
       <c r="V11" s="31"/>
-      <c r="W11" s="90" t="s">
+      <c r="W11" s="78" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1670,7 +1684,7 @@
       <c r="V12" s="40">
         <v>0.01</v>
       </c>
-      <c r="W12" s="91"/>
+      <c r="W12" s="79"/>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="42" t="s">
@@ -1682,7 +1696,9 @@
       <c r="C13" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D13" s="42"/>
+      <c r="D13" s="42" t="s">
+        <v>53</v>
+      </c>
       <c r="E13" s="42" t="s">
         <v>27</v>
       </c>
@@ -1731,7 +1747,7 @@
       </c>
       <c r="U13" s="42"/>
       <c r="V13" s="42"/>
-      <c r="W13" s="92"/>
+      <c r="W13" s="80"/>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
@@ -1743,7 +1759,9 @@
       <c r="C14" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="31"/>
+      <c r="D14" s="31" t="s">
+        <v>53</v>
+      </c>
       <c r="E14" s="31" t="s">
         <v>27</v>
       </c>
@@ -1790,7 +1808,7 @@
       </c>
       <c r="U14" s="31"/>
       <c r="V14" s="31"/>
-      <c r="W14" s="90" t="s">
+      <c r="W14" s="78" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1857,7 +1875,7 @@
       <c r="V15" s="40">
         <v>0.01</v>
       </c>
-      <c r="W15" s="91"/>
+      <c r="W15" s="79"/>
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="42" t="s">
@@ -1869,7 +1887,9 @@
       <c r="C16" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="42"/>
+      <c r="D16" s="42" t="s">
+        <v>53</v>
+      </c>
       <c r="E16" s="42" t="s">
         <v>27</v>
       </c>
@@ -1918,7 +1938,7 @@
       </c>
       <c r="U16" s="42"/>
       <c r="V16" s="42"/>
-      <c r="W16" s="92"/>
+      <c r="W16" s="80"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
@@ -1943,7 +1963,7 @@
       <c r="T17" s="14"/>
       <c r="U17" s="14"/>
       <c r="V17" s="14"/>
-      <c r="W17" s="87"/>
+      <c r="W17" s="84"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
@@ -1968,7 +1988,7 @@
       <c r="T18" s="15"/>
       <c r="U18" s="15"/>
       <c r="V18" s="21"/>
-      <c r="W18" s="88"/>
+      <c r="W18" s="85"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
@@ -1993,7 +2013,7 @@
       <c r="T19" s="23"/>
       <c r="U19" s="23"/>
       <c r="V19" s="23"/>
-      <c r="W19" s="89"/>
+      <c r="W19" s="86"/>
     </row>
     <row r="20" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30"/>
@@ -2018,7 +2038,7 @@
       <c r="T20" s="31"/>
       <c r="U20" s="31"/>
       <c r="V20" s="31"/>
-      <c r="W20" s="90"/>
+      <c r="W20" s="78"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
@@ -2043,7 +2063,7 @@
       <c r="T21" s="32"/>
       <c r="U21" s="32"/>
       <c r="V21" s="40"/>
-      <c r="W21" s="91"/>
+      <c r="W21" s="79"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" s="41"/>
@@ -2068,7 +2088,7 @@
       <c r="T22" s="42"/>
       <c r="U22" s="42"/>
       <c r="V22" s="42"/>
-      <c r="W22" s="92"/>
+      <c r="W22" s="80"/>
     </row>
     <row r="23" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="46"/>
@@ -2093,7 +2113,7 @@
       <c r="T23" s="47"/>
       <c r="U23" s="47"/>
       <c r="V23" s="47"/>
-      <c r="W23" s="78"/>
+      <c r="W23" s="87"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" s="53"/>
@@ -2118,7 +2138,7 @@
       <c r="T24" s="48"/>
       <c r="U24" s="48"/>
       <c r="V24" s="56"/>
-      <c r="W24" s="79"/>
+      <c r="W24" s="88"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" s="57"/>
@@ -2143,7 +2163,7 @@
       <c r="T25" s="58"/>
       <c r="U25" s="58"/>
       <c r="V25" s="58"/>
-      <c r="W25" s="80"/>
+      <c r="W25" s="89"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" s="62"/>
@@ -2168,7 +2188,7 @@
       <c r="T26" s="63"/>
       <c r="U26" s="63"/>
       <c r="V26" s="63"/>
-      <c r="W26" s="81"/>
+      <c r="W26" s="90"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" s="69"/>
@@ -2193,7 +2213,7 @@
       <c r="T27" s="64"/>
       <c r="U27" s="64"/>
       <c r="V27" s="72"/>
-      <c r="W27" s="82"/>
+      <c r="W27" s="91"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" s="73"/>
@@ -2218,19 +2238,19 @@
       <c r="T28" s="74"/>
       <c r="U28" s="74"/>
       <c r="V28" s="74"/>
-      <c r="W28" s="83"/>
+      <c r="W28" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="W26:W28"/>
+    <mergeCell ref="W11:W13"/>
+    <mergeCell ref="W8:W10"/>
     <mergeCell ref="W5:W7"/>
     <mergeCell ref="W2:W4"/>
     <mergeCell ref="W17:W19"/>
     <mergeCell ref="W20:W22"/>
     <mergeCell ref="W23:W25"/>
     <mergeCell ref="W14:W16"/>
-    <mergeCell ref="W26:W28"/>
-    <mergeCell ref="W11:W13"/>
-    <mergeCell ref="W8:W10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Correct the typo in storage setup file (electrolyte)
</commit_message>
<xml_diff>
--- a/scenario work/China/data/setup_storage_CHN.xlsx
+++ b/scenario work/China/data/setup_storage_CHN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakeri\Documents\Github\time_clustering\scenario work\China\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6969DCD-98DD-41F0-BFA1-7A7F0F561218}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEB8A7D1-ACED-48F0-AF4C-145985962CA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20235" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="storage" sheetId="20" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="75">
   <si>
     <t>technology</t>
   </si>
@@ -153,9 +153,6 @@
     <t>storage_phs</t>
   </si>
   <si>
-    <t>relation</t>
-  </si>
-  <si>
     <t>hydro_phs</t>
   </si>
   <si>
@@ -189,12 +186,6 @@
     <t>electr</t>
   </si>
   <si>
-    <t>electrolite</t>
-  </si>
-  <si>
-    <t>electorlite</t>
-  </si>
-  <si>
     <t>1.2</t>
   </si>
   <si>
@@ -265,6 +256,27 @@
   </si>
   <si>
     <t>Dis</t>
+  </si>
+  <si>
+    <t>relation_total_capacity</t>
+  </si>
+  <si>
+    <t>relation_activity_time</t>
+  </si>
+  <si>
+    <t>res_marg:1</t>
+  </si>
+  <si>
+    <t>tec_relation_from</t>
+  </si>
+  <si>
+    <t>oper_res:1/solar_curtailment_1:1/solar_curtailment_2:1/solar_curtailment_3:1/wind_curtailment_1:1/wind_curtailment_2:1/wind_curtailment_3:1</t>
+  </si>
+  <si>
+    <t>water_downstream/secondary</t>
+  </si>
+  <si>
+    <t>electrolyte</t>
   </si>
 </sst>
 </file>
@@ -536,6 +548,15 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -570,15 +591,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -884,10 +896,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F56DBD-A483-468D-94AB-6D22FF1A0021}">
-  <dimension ref="A1:W28"/>
+  <dimension ref="A1:Y28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,16 +917,16 @@
     <col min="13" max="13" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17.42578125" customWidth="1"/>
     <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="9.85546875" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8" customWidth="1"/>
-    <col min="22" max="22" width="7.42578125" customWidth="1"/>
-    <col min="23" max="23" width="35.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="9.85546875" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8" customWidth="1"/>
+    <col min="24" max="24" width="7.42578125" customWidth="1"/>
+    <col min="25" max="25" width="35.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
@@ -922,10 +934,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>5</v>
@@ -964,39 +976,45 @@
         <v>24</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="R1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="W1" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y1" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>27</v>
@@ -1005,7 +1023,7 @@
         <v>29</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>4</v>
@@ -1033,33 +1051,35 @@
       </c>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
-      <c r="R2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S2" s="27" t="s">
-        <v>38</v>
-      </c>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
       <c r="T2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="81" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="U2" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="84" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>27</v>
@@ -1096,35 +1116,37 @@
       </c>
       <c r="P3" s="9"/>
       <c r="Q3" s="9"/>
-      <c r="R3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="S3" s="12" t="s">
-        <v>36</v>
-      </c>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
       <c r="T3" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="U3" s="9">
+        <v>27</v>
+      </c>
+      <c r="U3" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="V3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="W3" s="9">
         <v>1</v>
       </c>
-      <c r="V3" s="12">
+      <c r="X3" s="12">
         <v>0.01</v>
       </c>
-      <c r="W3" s="82"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y3" s="85"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E4" s="9" t="s">
         <v>27</v>
@@ -1133,7 +1155,7 @@
         <v>29</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>4</v>
@@ -1151,7 +1173,7 @@
         <v>15</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
       <c r="N4" s="11" t="s">
         <v>26</v>
@@ -1161,33 +1183,39 @@
       </c>
       <c r="P4" s="9"/>
       <c r="Q4" s="9" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="R4" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="S4" s="12" t="s">
-        <v>37</v>
+        <v>70</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="T4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="U4" s="9"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="83"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="U4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="V4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="W4" s="9"/>
+      <c r="X4" s="12"/>
+      <c r="Y4" s="86"/>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E5" s="31" t="s">
         <v>27</v>
@@ -1196,22 +1224,22 @@
         <v>29</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H5" s="31" t="s">
         <v>4</v>
       </c>
       <c r="I5" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="J5" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="34" t="s">
-        <v>47</v>
-      </c>
       <c r="L5" s="31" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="M5" s="31" t="s">
         <v>9</v>
@@ -1220,37 +1248,39 @@
         <v>17</v>
       </c>
       <c r="O5" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P5" s="31"/>
       <c r="Q5" s="31"/>
-      <c r="R5" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="S5" s="36" t="s">
-        <v>39</v>
-      </c>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
       <c r="T5" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="U5" s="31"/>
-      <c r="V5" s="31"/>
-      <c r="W5" s="78" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="U5" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="V5" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="W5" s="31"/>
+      <c r="X5" s="31"/>
+      <c r="Y5" s="81" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D6" s="32" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E6" s="32" t="s">
         <v>27</v>
@@ -1265,7 +1295,7 @@
         <v>4</v>
       </c>
       <c r="I6" s="32" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="J6" s="32" t="s">
         <v>9</v>
@@ -1274,7 +1304,7 @@
         <v>17</v>
       </c>
       <c r="L6" s="32" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="M6" s="32" t="s">
         <v>9</v>
@@ -1283,39 +1313,41 @@
         <v>17</v>
       </c>
       <c r="O6" s="32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P6" s="32"/>
       <c r="Q6" s="32"/>
-      <c r="R6" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="S6" s="40" t="s">
-        <v>36</v>
-      </c>
+      <c r="R6" s="32"/>
+      <c r="S6" s="32"/>
       <c r="T6" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="U6" s="32">
+        <v>27</v>
+      </c>
+      <c r="U6" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="V6" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="W6" s="32">
         <v>1</v>
       </c>
-      <c r="V6" s="40">
+      <c r="X6" s="40">
         <v>0.01</v>
       </c>
-      <c r="W6" s="79"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y6" s="82"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="42" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="42" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E7" s="42" t="s">
         <v>27</v>
@@ -1324,13 +1356,13 @@
         <v>29</v>
       </c>
       <c r="G7" s="42" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="H7" s="42" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="42" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="J7" s="42" t="s">
         <v>9</v>
@@ -1339,46 +1371,52 @@
         <v>17</v>
       </c>
       <c r="L7" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M7" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N7" s="44" t="s">
         <v>17</v>
       </c>
       <c r="O7" s="42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P7" s="42"/>
       <c r="Q7" s="42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R7" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="S7" s="45" t="s">
-        <v>37</v>
+        <v>70</v>
+      </c>
+      <c r="S7" s="42" t="s">
+        <v>72</v>
       </c>
       <c r="T7" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="U7" s="42"/>
-      <c r="V7" s="42"/>
-      <c r="W7" s="80"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="U7" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="V7" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="W7" s="42"/>
+      <c r="X7" s="42"/>
+      <c r="Y7" s="83"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E8" s="31" t="s">
         <v>27</v>
@@ -1387,22 +1425,22 @@
         <v>29</v>
       </c>
       <c r="G8" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="H8" s="32" t="s">
         <v>4</v>
       </c>
       <c r="I8" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="K8" s="34" t="s">
-        <v>47</v>
-      </c>
       <c r="L8" s="31" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="M8" s="31" t="s">
         <v>9</v>
@@ -1411,37 +1449,39 @@
         <v>17</v>
       </c>
       <c r="O8" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P8" s="31"/>
       <c r="Q8" s="31"/>
-      <c r="R8" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="S8" s="36" t="s">
-        <v>39</v>
-      </c>
+      <c r="R8" s="31"/>
+      <c r="S8" s="31"/>
       <c r="T8" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="U8" s="31"/>
-      <c r="V8" s="31"/>
-      <c r="W8" s="78" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="U8" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="V8" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="W8" s="31"/>
+      <c r="X8" s="31"/>
+      <c r="Y8" s="81" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D9" s="32" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E9" s="32" t="s">
         <v>27</v>
@@ -1456,7 +1496,7 @@
         <v>4</v>
       </c>
       <c r="I9" s="32" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="J9" s="32" t="s">
         <v>9</v>
@@ -1465,7 +1505,7 @@
         <v>17</v>
       </c>
       <c r="L9" s="32" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="M9" s="32" t="s">
         <v>9</v>
@@ -1474,39 +1514,41 @@
         <v>17</v>
       </c>
       <c r="O9" s="32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P9" s="32"/>
       <c r="Q9" s="32"/>
-      <c r="R9" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="S9" s="40" t="s">
-        <v>36</v>
-      </c>
+      <c r="R9" s="32"/>
+      <c r="S9" s="32"/>
       <c r="T9" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="U9" s="32">
+        <v>27</v>
+      </c>
+      <c r="U9" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="V9" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="W9" s="32">
         <v>1</v>
       </c>
-      <c r="V9" s="40">
+      <c r="X9" s="40">
         <v>0.01</v>
       </c>
-      <c r="W9" s="79"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y9" s="82"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="42" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E10" s="42" t="s">
         <v>27</v>
@@ -1515,13 +1557,13 @@
         <v>29</v>
       </c>
       <c r="G10" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="32" t="s">
         <v>4</v>
       </c>
       <c r="I10" s="42" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="J10" s="42" t="s">
         <v>9</v>
@@ -1530,46 +1572,52 @@
         <v>17</v>
       </c>
       <c r="L10" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M10" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N10" s="44" t="s">
         <v>17</v>
       </c>
       <c r="O10" s="42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P10" s="42"/>
       <c r="Q10" s="42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R10" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="S10" s="45" t="s">
-        <v>37</v>
+        <v>70</v>
+      </c>
+      <c r="S10" s="42" t="s">
+        <v>72</v>
       </c>
       <c r="T10" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="U10" s="42"/>
-      <c r="V10" s="42"/>
-      <c r="W10" s="80"/>
-    </row>
-    <row r="11" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="U10" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="V10" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="W10" s="42"/>
+      <c r="X10" s="42"/>
+      <c r="Y10" s="83"/>
+    </row>
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E11" s="31" t="s">
         <v>27</v>
@@ -1578,22 +1626,22 @@
         <v>29</v>
       </c>
       <c r="G11" s="31" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H11" s="31" t="s">
         <v>4</v>
       </c>
       <c r="I11" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="K11" s="34" t="s">
-        <v>47</v>
-      </c>
       <c r="L11" s="31" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="M11" s="31" t="s">
         <v>9</v>
@@ -1602,37 +1650,39 @@
         <v>17</v>
       </c>
       <c r="O11" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P11" s="31"/>
       <c r="Q11" s="31"/>
-      <c r="R11" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="S11" s="36" t="s">
-        <v>39</v>
-      </c>
+      <c r="R11" s="31"/>
+      <c r="S11" s="31"/>
       <c r="T11" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="U11" s="31"/>
-      <c r="V11" s="31"/>
-      <c r="W11" s="78" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="U11" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="V11" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="W11" s="31"/>
+      <c r="X11" s="31"/>
+      <c r="Y11" s="81" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C12" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="32" t="s">
         <v>59</v>
-      </c>
-      <c r="D12" s="32" t="s">
-        <v>62</v>
       </c>
       <c r="E12" s="32" t="s">
         <v>27</v>
@@ -1647,7 +1697,7 @@
         <v>4</v>
       </c>
       <c r="I12" s="32" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="J12" s="32" t="s">
         <v>9</v>
@@ -1656,7 +1706,7 @@
         <v>17</v>
       </c>
       <c r="L12" s="32" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="M12" s="32" t="s">
         <v>9</v>
@@ -1665,39 +1715,41 @@
         <v>17</v>
       </c>
       <c r="O12" s="32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P12" s="32"/>
       <c r="Q12" s="32"/>
-      <c r="R12" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="S12" s="40" t="s">
-        <v>36</v>
-      </c>
+      <c r="R12" s="32"/>
+      <c r="S12" s="32"/>
       <c r="T12" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="U12" s="32">
+        <v>27</v>
+      </c>
+      <c r="U12" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="V12" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="W12" s="32">
         <v>1</v>
       </c>
-      <c r="V12" s="40">
+      <c r="X12" s="40">
         <v>0.01</v>
       </c>
-      <c r="W12" s="79"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y12" s="82"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="42" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="42" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E13" s="42" t="s">
         <v>27</v>
@@ -1706,13 +1758,13 @@
         <v>29</v>
       </c>
       <c r="G13" s="42" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H13" s="42" t="s">
         <v>4</v>
       </c>
       <c r="I13" s="42" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="J13" s="42" t="s">
         <v>9</v>
@@ -1721,46 +1773,52 @@
         <v>17</v>
       </c>
       <c r="L13" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M13" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N13" s="44" t="s">
         <v>17</v>
       </c>
       <c r="O13" s="42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P13" s="42"/>
       <c r="Q13" s="42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R13" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="S13" s="45" t="s">
-        <v>37</v>
+        <v>70</v>
+      </c>
+      <c r="S13" s="42" t="s">
+        <v>72</v>
       </c>
       <c r="T13" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="U13" s="42"/>
-      <c r="V13" s="42"/>
-      <c r="W13" s="80"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="U13" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="V13" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="W13" s="42"/>
+      <c r="X13" s="42"/>
+      <c r="Y13" s="83"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" s="31" t="s">
-        <v>53</v>
+        <v>66</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>60</v>
       </c>
       <c r="E14" s="31" t="s">
         <v>27</v>
@@ -1769,22 +1827,22 @@
         <v>29</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H14" s="31" t="s">
         <v>4</v>
       </c>
       <c r="I14" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="K14" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="J14" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="K14" s="34" t="s">
-        <v>47</v>
-      </c>
       <c r="L14" s="31" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="M14" s="31" t="s">
         <v>9</v>
@@ -1793,37 +1851,39 @@
         <v>17</v>
       </c>
       <c r="O14" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P14" s="31"/>
       <c r="Q14" s="31"/>
-      <c r="R14" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="S14" s="36" t="s">
-        <v>39</v>
-      </c>
+      <c r="R14" s="31"/>
+      <c r="S14" s="31"/>
       <c r="T14" s="31" t="s">
-        <v>48</v>
-      </c>
-      <c r="U14" s="31"/>
-      <c r="V14" s="31"/>
-      <c r="W14" s="78" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="U14" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="V14" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="W14" s="31"/>
+      <c r="X14" s="31"/>
+      <c r="Y14" s="81" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="D15" s="32" t="s">
         <v>60</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>63</v>
       </c>
       <c r="E15" s="32" t="s">
         <v>27</v>
@@ -1838,7 +1898,7 @@
         <v>4</v>
       </c>
       <c r="I15" s="32" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="J15" s="32" t="s">
         <v>9</v>
@@ -1847,7 +1907,7 @@
         <v>17</v>
       </c>
       <c r="L15" s="32" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="M15" s="32" t="s">
         <v>9</v>
@@ -1856,39 +1916,41 @@
         <v>17</v>
       </c>
       <c r="O15" s="32" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P15" s="32"/>
       <c r="Q15" s="32"/>
-      <c r="R15" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="S15" s="40" t="s">
-        <v>36</v>
-      </c>
+      <c r="R15" s="32"/>
+      <c r="S15" s="32"/>
       <c r="T15" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="U15" s="32">
+        <v>27</v>
+      </c>
+      <c r="U15" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="V15" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="W15" s="32">
         <v>1</v>
       </c>
-      <c r="V15" s="40">
+      <c r="X15" s="40">
         <v>0.01</v>
       </c>
-      <c r="W15" s="79"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y15" s="82"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="42" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="42" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="D16" s="42" t="s">
-        <v>53</v>
+        <v>67</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>60</v>
       </c>
       <c r="E16" s="42" t="s">
         <v>27</v>
@@ -1897,13 +1959,13 @@
         <v>29</v>
       </c>
       <c r="G16" s="42" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="H16" s="42" t="s">
         <v>4</v>
       </c>
       <c r="I16" s="42" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="J16" s="42" t="s">
         <v>9</v>
@@ -1912,35 +1974,41 @@
         <v>17</v>
       </c>
       <c r="L16" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M16" s="42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N16" s="44" t="s">
         <v>17</v>
       </c>
       <c r="O16" s="42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P16" s="42"/>
       <c r="Q16" s="42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="R16" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="S16" s="45" t="s">
-        <v>37</v>
+        <v>70</v>
+      </c>
+      <c r="S16" s="42" t="s">
+        <v>72</v>
       </c>
       <c r="T16" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="U16" s="42"/>
-      <c r="V16" s="42"/>
-      <c r="W16" s="80"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="U16" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="V16" s="42" t="s">
+        <v>45</v>
+      </c>
+      <c r="W16" s="42"/>
+      <c r="X16" s="42"/>
+      <c r="Y16" s="83"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
@@ -1959,13 +2027,15 @@
       <c r="P17" s="14"/>
       <c r="Q17" s="14"/>
       <c r="R17" s="14"/>
-      <c r="S17" s="28"/>
+      <c r="S17" s="14"/>
       <c r="T17" s="14"/>
-      <c r="U17" s="14"/>
+      <c r="U17" s="28"/>
       <c r="V17" s="14"/>
-      <c r="W17" s="84"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W17" s="14"/>
+      <c r="X17" s="14"/>
+      <c r="Y17" s="87"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
       <c r="B18" s="15"/>
       <c r="C18" s="15"/>
@@ -1984,13 +2054,15 @@
       <c r="P18" s="15"/>
       <c r="Q18" s="15"/>
       <c r="R18" s="15"/>
-      <c r="S18" s="21"/>
+      <c r="S18" s="15"/>
       <c r="T18" s="15"/>
-      <c r="U18" s="15"/>
-      <c r="V18" s="21"/>
-      <c r="W18" s="85"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U18" s="21"/>
+      <c r="V18" s="15"/>
+      <c r="W18" s="15"/>
+      <c r="X18" s="21"/>
+      <c r="Y18" s="88"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
@@ -2009,13 +2081,15 @@
       <c r="P19" s="23"/>
       <c r="Q19" s="23"/>
       <c r="R19" s="23"/>
-      <c r="S19" s="29"/>
+      <c r="S19" s="23"/>
       <c r="T19" s="23"/>
-      <c r="U19" s="23"/>
+      <c r="U19" s="29"/>
       <c r="V19" s="23"/>
-      <c r="W19" s="86"/>
-    </row>
-    <row r="20" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W19" s="23"/>
+      <c r="X19" s="23"/>
+      <c r="Y19" s="89"/>
+    </row>
+    <row r="20" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="30"/>
       <c r="B20" s="31"/>
       <c r="C20" s="31"/>
@@ -2034,13 +2108,15 @@
       <c r="P20" s="31"/>
       <c r="Q20" s="31"/>
       <c r="R20" s="31"/>
-      <c r="S20" s="36"/>
+      <c r="S20" s="31"/>
       <c r="T20" s="31"/>
-      <c r="U20" s="31"/>
+      <c r="U20" s="36"/>
       <c r="V20" s="31"/>
-      <c r="W20" s="78"/>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W20" s="31"/>
+      <c r="X20" s="31"/>
+      <c r="Y20" s="81"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="37"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
@@ -2059,13 +2135,15 @@
       <c r="P21" s="32"/>
       <c r="Q21" s="32"/>
       <c r="R21" s="32"/>
-      <c r="S21" s="40"/>
+      <c r="S21" s="32"/>
       <c r="T21" s="32"/>
-      <c r="U21" s="32"/>
-      <c r="V21" s="40"/>
-      <c r="W21" s="79"/>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U21" s="40"/>
+      <c r="V21" s="32"/>
+      <c r="W21" s="32"/>
+      <c r="X21" s="40"/>
+      <c r="Y21" s="82"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="41"/>
       <c r="B22" s="42"/>
       <c r="C22" s="42"/>
@@ -2084,13 +2162,15 @@
       <c r="P22" s="42"/>
       <c r="Q22" s="42"/>
       <c r="R22" s="42"/>
-      <c r="S22" s="45"/>
+      <c r="S22" s="42"/>
       <c r="T22" s="42"/>
-      <c r="U22" s="42"/>
+      <c r="U22" s="45"/>
       <c r="V22" s="42"/>
-      <c r="W22" s="80"/>
-    </row>
-    <row r="23" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W22" s="42"/>
+      <c r="X22" s="42"/>
+      <c r="Y22" s="83"/>
+    </row>
+    <row r="23" spans="1:25" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="46"/>
       <c r="B23" s="47"/>
       <c r="C23" s="47"/>
@@ -2109,13 +2189,15 @@
       <c r="P23" s="47"/>
       <c r="Q23" s="47"/>
       <c r="R23" s="47"/>
-      <c r="S23" s="52"/>
+      <c r="S23" s="47"/>
       <c r="T23" s="47"/>
-      <c r="U23" s="47"/>
+      <c r="U23" s="52"/>
       <c r="V23" s="47"/>
-      <c r="W23" s="87"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W23" s="47"/>
+      <c r="X23" s="47"/>
+      <c r="Y23" s="90"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="53"/>
       <c r="B24" s="48"/>
       <c r="C24" s="48"/>
@@ -2134,13 +2216,15 @@
       <c r="P24" s="48"/>
       <c r="Q24" s="48"/>
       <c r="R24" s="48"/>
-      <c r="S24" s="56"/>
+      <c r="S24" s="48"/>
       <c r="T24" s="48"/>
-      <c r="U24" s="48"/>
-      <c r="V24" s="56"/>
-      <c r="W24" s="88"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U24" s="56"/>
+      <c r="V24" s="48"/>
+      <c r="W24" s="48"/>
+      <c r="X24" s="56"/>
+      <c r="Y24" s="91"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="57"/>
       <c r="B25" s="58"/>
       <c r="C25" s="58"/>
@@ -2159,13 +2243,15 @@
       <c r="P25" s="58"/>
       <c r="Q25" s="58"/>
       <c r="R25" s="58"/>
-      <c r="S25" s="61"/>
+      <c r="S25" s="58"/>
       <c r="T25" s="58"/>
-      <c r="U25" s="58"/>
+      <c r="U25" s="61"/>
       <c r="V25" s="58"/>
-      <c r="W25" s="89"/>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W25" s="58"/>
+      <c r="X25" s="58"/>
+      <c r="Y25" s="92"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="62"/>
       <c r="B26" s="63"/>
       <c r="C26" s="63"/>
@@ -2184,13 +2270,15 @@
       <c r="P26" s="63"/>
       <c r="Q26" s="63"/>
       <c r="R26" s="63"/>
-      <c r="S26" s="68"/>
+      <c r="S26" s="63"/>
       <c r="T26" s="63"/>
-      <c r="U26" s="63"/>
+      <c r="U26" s="68"/>
       <c r="V26" s="63"/>
-      <c r="W26" s="90"/>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="W26" s="63"/>
+      <c r="X26" s="63"/>
+      <c r="Y26" s="78"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="69"/>
       <c r="B27" s="64"/>
       <c r="C27" s="64"/>
@@ -2209,13 +2297,15 @@
       <c r="P27" s="64"/>
       <c r="Q27" s="64"/>
       <c r="R27" s="64"/>
-      <c r="S27" s="72"/>
+      <c r="S27" s="64"/>
       <c r="T27" s="64"/>
-      <c r="U27" s="64"/>
-      <c r="V27" s="72"/>
-      <c r="W27" s="91"/>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U27" s="72"/>
+      <c r="V27" s="64"/>
+      <c r="W27" s="64"/>
+      <c r="X27" s="72"/>
+      <c r="Y27" s="79"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="73"/>
       <c r="B28" s="74"/>
       <c r="C28" s="74"/>
@@ -2234,23 +2324,25 @@
       <c r="P28" s="74"/>
       <c r="Q28" s="74"/>
       <c r="R28" s="74"/>
-      <c r="S28" s="77"/>
+      <c r="S28" s="74"/>
       <c r="T28" s="74"/>
-      <c r="U28" s="74"/>
+      <c r="U28" s="77"/>
       <c r="V28" s="74"/>
-      <c r="W28" s="92"/>
+      <c r="W28" s="74"/>
+      <c r="X28" s="74"/>
+      <c r="Y28" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="W26:W28"/>
-    <mergeCell ref="W11:W13"/>
-    <mergeCell ref="W8:W10"/>
-    <mergeCell ref="W5:W7"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="W17:W19"/>
-    <mergeCell ref="W20:W22"/>
-    <mergeCell ref="W23:W25"/>
-    <mergeCell ref="W14:W16"/>
+    <mergeCell ref="Y26:Y28"/>
+    <mergeCell ref="Y11:Y13"/>
+    <mergeCell ref="Y8:Y10"/>
+    <mergeCell ref="Y5:Y7"/>
+    <mergeCell ref="Y2:Y4"/>
+    <mergeCell ref="Y17:Y19"/>
+    <mergeCell ref="Y20:Y22"/>
+    <mergeCell ref="Y23:Y25"/>
+    <mergeCell ref="Y14:Y16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>